<commit_message>
Now passing all tests except `escape`
</commit_message>
<xml_diff>
--- a/test/general_copy_2.xlsx
+++ b/test/general_copy_2.xlsx
@@ -13,7 +13,7 @@
     <workbookView xWindow="2970" yWindow="3000" windowWidth="28800" windowHeight="15435" tabRatio="500" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="general" sheetId="1" r:id="rId1"/>
+    <sheet name="renamed_sheet" sheetId="1" r:id="rId1"/>
     <sheet name="table3" sheetId="4" r:id="rId2"/>
     <sheet name="table4" sheetId="5" r:id="rId3"/>
     <sheet name="table" sheetId="2" r:id="rId4"/>
@@ -597,87 +597,6 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>102.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>30422</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.82291666666666663</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3">
-        <v>43206.805447106482</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="5">
-        <v>-220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8">
-        <v>-2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9">
-        <v>100000000000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10">
-        <f>-100000000000000</f>
-        <v>-100000000000000</v>
-      </c>
-    </row>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
         <v>59</v>
       </c>
       <c r="B1" t="s">
@@ -825,104 +744,6 @@
         <v>20</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C4:C5" si="0">VLOOKUP(B4,$F$3:$G$5,2,FALSE)</f>
-        <v>name2</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:D5" si="1">VLOOKUP(B4,$I$3:$J$5,2,FALSE)</f>
-        <v>200</v>
-      </c>
-      <c r="F4">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4">
-        <v>20</v>
-      </c>
-      <c r="J4">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>30</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>name3</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>300</v>
-      </c>
-      <c r="F5">
-        <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5">
-        <v>30</v>
-      </c>
-      <c r="J5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3" t="str">
-        <f>VLOOKUP(B3,$F$3:$G$5,2,FALSE)</f>
-        <v>name1</v>
-      </c>
-      <c r="D3">
-        <f>VLOOKUP(B3,$I$3:$J$5,2,FALSE)</f>
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3">
-        <v>10</v>
-      </c>
-      <c r="J3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>20</v>
-      </c>
-      <c r="C4" t="str">
         <v>name2</v>
       </c>
       <c r="D4">
@@ -1018,45 +839,6 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" t="s">
-        <v>58</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1072,40 +854,6 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="str">
-        <f>LOCAL_NAME</f>
-        <v>out there in the cold</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <f>CONST_INT</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>LOCAL_INT</f>
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D4" t="str">
-        <f>LOCAL_REF</f>
-        <v>local</v>
-      </c>
-      <c r="E4" t="str">
-        <f>LOCAL_REF</f>
-        <v>reference</v>
-      </c>
-    </row>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="str">
         <f>LOCAL_NAME</f>
@@ -1163,71 +911,6 @@
         <v>48</v>
       </c>
       <c r="E2">
-        <f t="array" ref="E2:F2">LOCAL_REF</f>
-        <v>10</v>
-      </c>
-      <c r="F2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8">
-        <f>CONST_INT</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="str">
-        <f>LOCAL_NAME</f>
-        <v>Hey You</v>
-      </c>
-      <c r="B9">
-        <f>CONST_DATE</f>
-        <v>43383</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f>LOCAL_INT</f>
-        <v>1000</v>
-      </c>
-      <c r="B10">
-        <f>CONST_FLOAT</f>
-        <v>10.199999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2">
         <v>10</v>
       </c>
       <c r="F2">
@@ -1299,89 +982,7 @@
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>102.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>30422</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.82291666666666663</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3">
-        <v>43206.805447106482</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="5">
-        <v>-220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8">
-        <v>-2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9">
-        <v>100000000000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10">
-        <f>-100000000000000</f>
-        <v>-100000000000000</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1404,92 +1005,6 @@
         <v>63</v>
       </c>
     </row>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>102.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>30422</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.82291666666666663</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3">
-        <v>43206.805447106482</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="5">
-        <v>-220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8">
-        <v>-2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9">
-        <v>100000000000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10">
-        <f>-100000000000000</f>
-        <v>-100000000000000</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1506,87 +1021,6 @@
     <row r="1" spans="1:2">
       <c r="B1" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>102.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1">
-        <v>30422</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.82291666666666663</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3">
-        <v>43206.805447106482</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="5">
-        <v>-220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8">
-        <v>-2000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9">
-        <v>100000000000000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10">
-        <f>-100000000000000</f>
-        <v>-100000000000000</v>
       </c>
     </row>
   </sheetData>
@@ -1647,49 +1081,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1731,32 +1122,6 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
-        <v>34</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1807,204 +1172,6 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4">
-        <f>B3+1</f>
-        <v>2</v>
-      </c>
-      <c r="D4" s="1">
-        <f>D3+1</f>
-        <v>43212</v>
-      </c>
-      <c r="F4">
-        <v>0.27939873773400004</v>
-      </c>
-      <c r="H4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5">
-        <f t="shared" ref="B5:B10" si="0">B4+1</f>
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" ref="D5:D10" si="1">D4+1</f>
-        <v>43213</v>
-      </c>
-      <c r="F5">
-        <v>9.5059167683513524E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" si="1"/>
-        <v>43214</v>
-      </c>
-      <c r="F6">
-        <v>7.4402306732486267E-2</v>
-      </c>
-      <c r="H6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" si="1"/>
-        <v>43215</v>
-      </c>
-      <c r="F7">
-        <v>0.82422780912015003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="1"/>
-        <v>43216</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8">
-        <v>0.62058835778747101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="1">
-        <f t="shared" si="1"/>
-        <v>43217</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9">
-        <v>0.91741510177329644</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="1">
-        <f t="shared" si="1"/>
-        <v>43218</v>
-      </c>
-      <c r="F10">
-        <v>0.67496048826901078</v>
-      </c>
-      <c r="H10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1">
-        <v>43211</v>
-      </c>
-      <c r="F3">
-        <v>0.20011323191065111</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="4">
         <v>18</v>
       </c>
@@ -2218,43 +1385,6 @@
         <v>28</v>
       </c>
     </row>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2314,36 +1444,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2394,41 +1494,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2479,41 +1544,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>